<commit_message>
new and updated workflows
</commit_message>
<xml_diff>
--- a/data/fuel supply.xlsx
+++ b/data/fuel supply.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lauri\Documents\RPackages\china_co2\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F186025F-9CE6-474D-B240-E5F665C9F3A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09CB81F2-8681-46B1-BB55-D027E94E9AE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Output_ Natural Crude Oil_ YTD" sheetId="1" r:id="rId1"/>
+    <sheet name="Output_Natural Crude Oil_YTD" sheetId="1" r:id="rId1"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId2"/>
@@ -48,7 +48,7 @@
             <sz val="9"/>
             <rFont val="宋体"/>
           </rPr>
-          <t>UEsDBBQACAgIAK1pD1cAAAAAAAAAAAAAAAABAAAAMM2Y7Y/URBjA77N/RdMvQnKTTGemM22/wR2nhJdDWEkMIWY683Svoduu7VS5kEs0gUAwkUtQv2CCRowao4KgvEQk8W9h9/C/cLovx8HtHWvgTvbLdp55e/p7XuaZHpjfP/PGzMzMORfOdovSzBV5krbd6JyrIZF1Zg7LvF3LNriRC7k76+q06mZy+UihG5HuHMx1qqRJi6YzrfZVyo1MWUPTeDvVsD+T+ZmhaGV2tEkrNRksdgeT7E4yywaSAxl0IDeVGyUyq+wKqqhzUy6vtzVUqkxH84abJCV8UEOultd31XaJNEmhHEsq2elmsN6CDJQBPdjxECwfTivjRqfcEipTlHBUdsAdLmv/6jw1bqOHboRamuavKupSNQ91t5HMN9LT6+LRNkbG2XCxsfLNWtW4e8PUMZoOmDK18E6dc9+3nXI+bQ8mkFk3hnaaDwe7XhiEmJCgUWvJ2gaOgypKbeedHikauScwJgJTYcdAPlTCXaxNtzaRc1SaupSZM1fWGpzFNIuc91rzg5HvNm9rd8D255gir9yBwWSuQa+/Bpw1pVSmJdsbTeBGbNZtl0XdHXSMxp4BaxaXcRV7WgqdYBF7nAR+SIivaEgTzlTo213yZ3XcpNvIOOv0hoo+vnext/qDuzL7ImKhjz3qvZAYoXwjsXdqaT3JLDtF4hzsNH5bTVBt57CFXkjDQPix9CWlvuCUYuwB92PKIKBPsZ0ssroD26v5UgQJxhSLaQgyspHg3FKay8iZoN9CmqfVEuhGRedYWehamcrZ01oCZ662mnaqN50TxqaVytjskjXPuZal3rvj2H1KREziAIWaEsRCTVDsEYWE1phTT/mEi6foH9/7uXftYfTk0bXelW/7X9z85+KVqH9ptXf1k/5v9/f0f7/bu3Db9vT+Or83Wrvz65Nfvul9/OdGc2xIDjtiD39bexw4+9rbIxaBBIAYxUnMEcMBQSERHiKc40R6SiolN9mjd/HBbtpjqgzjM+s5LJguPsZZ+i1ZTSLsdNIss6eg0/n79qvC7LEw0RTFWANiCfeQZEIjonnCfettWJHt3b5348e183/0b34+FdgHj9Z++rT/5f21W7enwGuPvGkSOGbeBLzPn3y7xlQQjqkXciRCIRCjOkaSSI4SIQVo8DxMkk1MHz/4/rWgadMLZdvQtElCQVWlebtx3GO2eCkyqDubyJpBYfgKaEqsWEh1ggCETcw08JHUhKGYaortK2mi+JY0P7tu4793+eve3e+a9hRMp4v7KVD6nmdja1Lcj1Eelx85c4W0Z3WrMHLnKwsZJhji0Ee2ELMpVXBho14JRCAgiWCaMqG2Ibl24UbUW71kAT7DsStLW3kftIoJHPDA35Wkij1BBaMT4E6u3ixlx+JzDqdtqwzsaCERxNySUAg49RHzE4lCHGIkfO6D4jwgsNlfn8moFnTvyuUnN1YHxB9e7X916XnUJOBcvDzpaa8UE8uJsRvbvFpkaQ477r+eohh4TJAHzLP+i21exZQhSgHHkoHNruFW/tu/9dBmgld69k8NL9wG3nwK9ma6KxcLnxAqMUiUxGFg8THf1lZAEPWZ1iEV3BewJb7rd/4vfP6kKB/jOwRlUcEu+F5AE5xwYc/0xIY2i6VAgS/tE/gUAgUs5FueQjaM/yM8y8CkHVgo7XInwBh72jYfTNQSqDMnZZbqsdqZrMxi3OBlw0ZrudsokDVSKD8cfKBpEBRxtVAWncElwqPY89hQaAv60uwzm+StYigKrKgxQBfKtNCj1btmoc6yYwORu7LyL1BLBwg3LV55OgUAAEwSAAA=</t>
+          <t>UEsDBBQACAgIAO5YL1cAAAAAAAAAAAAAAAABAAAAMM2Y7Y/URBjA77N/RdMvYnKTTGemM+1+gztOCSeHsJIYQsx05uleQ7dd26lyIZdoAoFgIpegfsEEjRg1RgVBeYlI4t/C7uF/4XTf7rjbO9bAneyX7TzTzjz9Pa/Tw/OHZl6bmZk578K5Tl6YuTyLk5bbOO9qiGWVmkWZtSrZArfhQubOujopO6lceTvXtUi3j2Q6UdIkeT2ZlAdL5TZMUUE9eCvRcCiV2dmRqCphscpk4TZimZawOjvctZmYFJY6/VXs1jJN+5LDKbQhM+Xw9llX5VVmipXxWEOpimT43GCLuIAPKsjUylgNbZdI4gSKkaSU7U4K4xGkoAzo/o5HYWUxKY3bOO0WUJq8gGOyDe5gWftXZYlxaz10LdTS1H9lXhWqvqg6tWS+lp4Zi4fbGBmlg8VGytdrlWMyG4/2JRZNG0yRWJqnz7vv20k5n7T6D5BZN4JWkg1udr0wCDEhwUithnsSYyIwFVYC2WBLd6kynco0nGPSVIVMnbmi0uAsJWnDea8537/z3frd7HrY/hyTZ6XbN4/MNOix0nDOFFKZpmxtBu422KzbKvKq058Y3nsWrBFcxlXkaSl0jEXkcRL4ISG+oiGNOVOhb3fJntVxm25DU4xZDRR9cv9Sd+0Hd3X2eXxCH3vU28KHUL6ZzzuVtF5iVpw8do60a58sJyiyd5BCL6RhIPxI+pJSX3BKMfaA+xFlENANSKfytGrD7mq+EC+CMcViwGvZBj+cAJUX9uVOn9lCkJHNBOeWk0w2nAn6LSRZUi6DrlV0jhe5rpQpnQPNZXDmKqtpu3zdOWlsDimNTSVpfZ1pWeg39hy7T4mISBSgUFOCWKgJijyikNAac+opn3Cxgf7J/Z+71x81nj6+3r36be+LW/9cutroXV7rXvuk99uDA73f73Uv3rEz3b8uvNFYv/vr01++6X7852ZzbAr8PbGHv6s9Dp975e0RiUACQISiOOKI4YCgkAgPEc5xLD0llZLb7NG99HA/7bE5n+xoD59Zz2HBdPExyslvynISYaedpKmtcE777zsvC7PHwlhTFGENiMXcQ5IJjYjmMfett2FFdnf77s0f1y/80bv1+VRgHz5e/+nT3pcP1m/fmQKvLWfPw9svcMybgHdrnds3poJwTL2QIxEKgRjVEZJEchQLKUCD52ESb2P65OH3rwRNm14o24WmTRIKyjLJWrXjHreNSZ5C1d5G1vS7wJdAU2LFQqpjBCBsYqaBj6QmDEVUU2xfSRPFd6T52Q0b/90rX3fvfVePp2A6XdxPgdL3PBtbk+J+hPKE/MiZy6Wt1c3cyL3vLGQYY4hCH9m2y6ZUwYWNeiUQgYDEgmnKhNqF5PrFm43u2mUL8BmOHVnYrvqIVUzggAf+viRV7AkqGJ0Ad3L3Zik7Fp+zmLSsMrCnjUQQcUtCIeDUR8yPJQpxiJHwuQ+K84DAdn99JqNa0N2rV57eXOsTf3St99XlrahJwLl4cdIbx4Xn5NdJ7cTIjW1ezdMkgz33X09RDDwiyAPmWf/FNq9iyhClgCPJwGbXcCf/7d1+ZDPBS639U8MLd4E3n4A9de7LwcInhEoMEsVRGFh8zLe9FRBEfaZ1SAX3BeyI78bd/wufPynKR/iOQpGXsA++F9AYx1zYmh7b0GaRFCjwpb0Cn0KggIV8xypkw/g/wrMMTNKGhcIudxKMsdW2/hiilkGdPSXTRI/UTmVplqIaLxsMmiudWoG0lkLxYf9rTI0gj8qFIm/3DxEexZ7HBkLb0BfmoNkmb+YDUWBFtQE6UCS5Hq7eMQtVmh7vi9zV1X8BUEsHCIkwEWhLBQAAORIAAA==</t>
         </r>
       </text>
     </comment>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="49">
   <si>
     <t>Name</t>
   </si>
@@ -158,25 +158,25 @@
     <t>Time Period</t>
   </si>
   <si>
-    <t>1989-02:2023-07</t>
+    <t>1989-02:2023-08</t>
+  </si>
+  <si>
+    <t>1995-01:2023-08</t>
+  </si>
+  <si>
+    <t>2003-07:2023-08</t>
   </si>
   <si>
     <t>1995-01:2023-07</t>
   </si>
   <si>
-    <t>2003-07:2023-07</t>
-  </si>
-  <si>
-    <t>1995-01:2023-06</t>
+    <t>1989-01:2023-08</t>
   </si>
   <si>
     <t>1989-01:2023-07</t>
   </si>
   <si>
-    <t>1989-01:2023-06</t>
-  </si>
-  <si>
-    <t>1989-02:2023-06</t>
+    <t>1989-02:2023-07</t>
   </si>
   <si>
     <t>Source</t>
@@ -194,19 +194,16 @@
     <t>Update</t>
   </si>
   <si>
-    <t>2023-08-15</t>
+    <t>2023-09-15</t>
   </si>
   <si>
-    <t>2023-08-08</t>
+    <t>2023-09-07</t>
   </si>
   <si>
-    <t>2023-07-25</t>
+    <t>2023-08-23</t>
   </si>
   <si>
-    <t>2023-07-17</t>
-  </si>
-  <si>
-    <t>2023-07-19</t>
+    <t>2023-08-16</t>
   </si>
 </sst>
 </file>
@@ -607,7 +604,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M423"/>
+  <dimension ref="A1:M424"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -897,13 +894,13 @@
         <v>46</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:13">
@@ -17885,39 +17882,80 @@
         <v>45138</v>
       </c>
       <c r="B423" s="5">
-        <v>12237</v>
+        <v>12236.6</v>
       </c>
       <c r="C423" s="5">
-        <v>32575.200000000001</v>
+        <v>32575.000000000004</v>
       </c>
       <c r="D423" s="5">
-        <v>2701.3</v>
+        <v>2701</v>
       </c>
       <c r="E423" s="5">
-        <v>3661.6</v>
+        <v>3662</v>
       </c>
       <c r="F423" s="5">
-        <v>0</v>
+        <v>929.86688300000003</v>
       </c>
       <c r="G423" s="5">
-        <v>1340</v>
+        <v>1340.4</v>
       </c>
       <c r="H423" s="5">
-        <v>426710000</v>
+        <v>426708000</v>
       </c>
       <c r="I423" s="5">
-        <v>0</v>
+        <v>267182</v>
       </c>
       <c r="J423" s="5">
         <v>3926</v>
       </c>
       <c r="K423" s="5">
-        <v>0</v>
+        <v>9224.2999999999993</v>
       </c>
       <c r="L423" s="5">
-        <v>0</v>
+        <v>12531.3</v>
       </c>
       <c r="M423" s="5">
+        <v>2713.7</v>
+      </c>
+    </row>
+    <row r="424" spans="1:13">
+      <c r="A424" s="4">
+        <v>45169</v>
+      </c>
+      <c r="B424" s="5">
+        <v>13984.799800000001</v>
+      </c>
+      <c r="C424" s="5">
+        <v>37855.4</v>
+      </c>
+      <c r="D424" s="5">
+        <v>3055</v>
+      </c>
+      <c r="E424" s="5">
+        <v>4250.7</v>
+      </c>
+      <c r="F424" s="5">
+        <v>0</v>
+      </c>
+      <c r="G424" s="5">
+        <v>1521.4662000000001</v>
+      </c>
+      <c r="H424" s="5">
+        <v>491401453</v>
+      </c>
+      <c r="I424" s="5">
+        <v>0</v>
+      </c>
+      <c r="J424" s="5">
+        <v>4433.2999999999993</v>
+      </c>
+      <c r="K424" s="5">
+        <v>0</v>
+      </c>
+      <c r="L424" s="5">
+        <v>0</v>
+      </c>
+      <c r="M424" s="5">
         <v>0</v>
       </c>
     </row>

</xml_diff>